<commit_message>
Excel update to binary student id
</commit_message>
<xml_diff>
--- a/Data/dta_student_id.xlsx
+++ b/Data/dta_student_id.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\PROYECTO FINAL\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\PROYECTOS\PYTHON\ESEN\2024\PROYECTO FINAL\IDS-Proyecto-Final\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3828DA-004D-47A0-95F9-9BAD9F642A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAFEEA3-157D-4138-A80D-336569BEA32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student_IDs" sheetId="1" r:id="rId1"/>
@@ -25,43 +25,140 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>André</t>
-  </si>
-  <si>
     <t>Scholarship</t>
   </si>
   <si>
     <t>Student ID</t>
   </si>
   <si>
-    <t>Dana</t>
-  </si>
-  <si>
-    <t>Oscar</t>
-  </si>
-  <si>
-    <t>Tiffany</t>
-  </si>
-  <si>
-    <t>Debbie</t>
+    <t>st1</t>
+  </si>
+  <si>
+    <t>st2</t>
+  </si>
+  <si>
+    <t>st3</t>
+  </si>
+  <si>
+    <t>st4</t>
+  </si>
+  <si>
+    <t>st5</t>
+  </si>
+  <si>
+    <t>st6</t>
+  </si>
+  <si>
+    <t>st7</t>
+  </si>
+  <si>
+    <t>st8</t>
+  </si>
+  <si>
+    <t>st9</t>
+  </si>
+  <si>
+    <t>st10</t>
+  </si>
+  <si>
+    <t>st11</t>
+  </si>
+  <si>
+    <t>st12</t>
+  </si>
+  <si>
+    <t>st13</t>
+  </si>
+  <si>
+    <t>st14</t>
+  </si>
+  <si>
+    <t>st15</t>
+  </si>
+  <si>
+    <t>st16</t>
+  </si>
+  <si>
+    <t>st17</t>
+  </si>
+  <si>
+    <t>st18</t>
+  </si>
+  <si>
+    <t>st19</t>
+  </si>
+  <si>
+    <t>st20</t>
+  </si>
+  <si>
+    <t>st21</t>
+  </si>
+  <si>
+    <t>st22</t>
+  </si>
+  <si>
+    <t>st23</t>
+  </si>
+  <si>
+    <t>st24</t>
+  </si>
+  <si>
+    <t>st25</t>
+  </si>
+  <si>
+    <t>st26</t>
+  </si>
+  <si>
+    <t>st27</t>
+  </si>
+  <si>
+    <t>st28</t>
+  </si>
+  <si>
+    <t>st29</t>
+  </si>
+  <si>
+    <t>st30</t>
+  </si>
+  <si>
+    <t>st31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,21 +181,100 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -125,7 +301,24 @@
       <bagId>2</bagId>
     </a>
   </bag>
+  <bag type="DXFComplements" extRef="DXFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
 </FeaturePropertyBags>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC65E24D-61B9-40A1-8B72-8B616B14DD6D}" name="Table1" displayName="Table1" ref="A1:C32" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C32" xr:uid="{CC65E24D-61B9-40A1-8B72-8B616B14DD6D}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0E81ACF5-40E2-486C-82A5-6033BB4AD773}" name="Student ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{9D57861C-2609-461F-946A-9F0FD2E5961A}" name="Name" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{F773E513-E77C-4732-B160-BB53D9D780AE}" name="Scholarship" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -391,44 +584,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>20245305</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C2" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>20245335</v>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -437,9 +631,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>20235899</v>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -448,9 +642,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>20245430</v>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -459,9 +653,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>20245476</v>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -470,8 +664,298 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>110</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>111</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1001</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1010</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1011</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1100</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1101</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1110</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1111</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>10001</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>10010</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>10011</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>10100</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>10101</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>10110</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>10111</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>11000</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>11001</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>11010</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>11011</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>11100</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>11101</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>11110</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>11111</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>